<commit_message>
Completed CF09_USTC and updated storyMap
</commit_message>
<xml_diff>
--- a/docs/storyMap.xlsx
+++ b/docs/storyMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2020\CEN3031\project\career-finder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB89231F-F16E-4015-9F7D-E2C88912328B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99E1691-55CD-450C-B901-C2E812B7A119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="careerFindStoryMap" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={EC7DB265-F8E0-4255-88FD-7E3B798F812B}</author>
+  </authors>
+  <commentList>
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{EC7DB265-F8E0-4255-88FD-7E3B798F812B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    userRequirements &gt; 1. Base System: A content management system allowing users to … read… celebrity names, articles, photos.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="94">
   <si>
@@ -322,7 +340,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +384,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -877,6 +901,9 @@
     <xf numFmtId="1" fontId="0" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -891,9 +918,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,6 +934,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Caplin,Robert O,II" id="{AEABF0B4-0D92-49F5-9F95-0526D087F34F}" userId="Caplin,Robert O,II" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1173,12 +1203,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H7" dT="2020-02-29T17:07:01.72" personId="{AEABF0B4-0D92-49F5-9F95-0526D087F34F}" id="{EC7DB265-F8E0-4255-88FD-7E3B798F812B}">
+    <text>userRequirements &gt; 1. Base System: A content management system allowing users to … read… celebrity names, articles, photos.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1290,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="5"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="85" t="s">
+      <c r="F4" s="86" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -1272,7 +1310,7 @@
       <c r="C5" s="12"/>
       <c r="D5" s="5"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="85"/>
+      <c r="F5" s="86"/>
       <c r="G5" s="9" t="s">
         <v>90</v>
       </c>
@@ -1290,7 +1328,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="5"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="85"/>
+      <c r="F6" s="86"/>
       <c r="G6" s="9" t="s">
         <v>16</v>
       </c>
@@ -1308,7 +1346,7 @@
       <c r="C7" s="12"/>
       <c r="D7" s="5"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="85"/>
+      <c r="F7" s="86"/>
       <c r="G7" s="9" t="s">
         <v>17</v>
       </c>
@@ -1342,7 +1380,7 @@
       <c r="C9" s="12"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="86" t="s">
+      <c r="F9" s="87" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="8"/>
@@ -1362,7 +1400,7 @@
       <c r="C10" s="12"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="86"/>
+      <c r="F10" s="87"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="10" t="s">
@@ -1378,7 +1416,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="86"/>
+      <c r="F11" s="87"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="10" t="s">
@@ -1394,7 +1432,7 @@
       <c r="C12" s="12"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="86"/>
+      <c r="F12" s="87"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="10" t="s">
@@ -1410,7 +1448,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="86"/>
+      <c r="F13" s="87"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="10" t="s">
@@ -1426,7 +1464,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="86"/>
+      <c r="F14" s="87"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="10" t="s">
@@ -1442,7 +1480,7 @@
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="87" t="s">
+      <c r="F15" s="88" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="13" t="s">
@@ -1462,7 +1500,7 @@
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
-      <c r="F16" s="87"/>
+      <c r="F16" s="88"/>
       <c r="G16" s="13" t="s">
         <v>30</v>
       </c>
@@ -1480,7 +1518,7 @@
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
-      <c r="F17" s="87"/>
+      <c r="F17" s="88"/>
       <c r="G17" s="13" t="s">
         <v>31</v>
       </c>
@@ -1496,7 +1534,7 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="88" t="s">
+      <c r="F18" s="89" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="18"/>
@@ -1514,7 +1552,7 @@
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
-      <c r="F19" s="88"/>
+      <c r="F19" s="89"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
@@ -1530,7 +1568,7 @@
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
-      <c r="F20" s="88"/>
+      <c r="F20" s="89"/>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
@@ -1546,7 +1584,7 @@
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="84" t="s">
+      <c r="F21" s="85" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="23"/>
@@ -1574,7 +1612,7 @@
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
-      <c r="F22" s="84"/>
+      <c r="F22" s="85"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="24" t="s">
@@ -1600,7 +1638,7 @@
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="84"/>
+      <c r="F23" s="85"/>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
@@ -1624,7 +1662,7 @@
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="84"/>
+      <c r="F24" s="85"/>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
@@ -1652,6 +1690,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1659,7 +1698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADC453F-97E4-4EC8-8383-D8BA2226CD2D}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -1723,7 +1762,7 @@
       <c r="C2" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="89">
+      <c r="D2" s="84">
         <f xml:space="preserve"> SUM($H2:$T2)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updates to storyMap while populating pivotal
</commit_message>
<xml_diff>
--- a/docs/storyMap.xlsx
+++ b/docs/storyMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2020\CEN3031\project\career-finder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99E1691-55CD-450C-B901-C2E812B7A119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F685476-4F6D-49E2-A8B3-266D280975B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>Theme: Progress Tracker</t>
   </si>
   <si>
-    <t>As a Counselor I want to manage (CRUD) careeers (name, salary, description, keyword associations) displayed on the site.</t>
-  </si>
-  <si>
     <t>As a Counselor I want to manage (CRUD) Day-In-the-Life articles that are associated with careers.</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>As a Student I want to answer a chat prompt after logging into the site and receive a career cluster recommendation based on parsed keywords in my response.</t>
   </si>
   <si>
-    <t>As a Student I want to my response to be logged if it does not contain any known keywords so that my Counselor can improve the system.</t>
-  </si>
-  <si>
     <t>As a Student I want recommended career clusters to be placed in a queue so that I can remember to visit them.</t>
   </si>
   <si>
@@ -327,20 +321,26 @@
     <t>As a Counselor I want to manage (CRUD) the keywords (name, type: subject, interest) used to associate career clusters, careers, and celebrities.</t>
   </si>
   <si>
-    <t>As a User after clicking on a career name I want to see base career data (name, salary, key subjects, description) and keyword-associated content links presneted on a page.</t>
-  </si>
-  <si>
     <t>As a Counselor I want to manage (CRUD) the carrer clusters ( name, icon, keyword associations) displayed on the site.</t>
   </si>
   <si>
     <t>API</t>
+  </si>
+  <si>
+    <t>As a Counselor I want to manage (CRUD) careers (name, salary, description, keyword associations) displayed on the site.</t>
+  </si>
+  <si>
+    <t>As a User after clicking on a career name I want to see base career data (name, salary, key subjects, description) and keyword-associated content links presented on a page.</t>
+  </si>
+  <si>
+    <t>As a Student I want my response to be logged if it does not contain any known keywords so that my Counselor can improve the system.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,12 +384,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1215,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1294,10 +1288,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -1312,10 +1306,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="86"/>
       <c r="G5" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -1330,10 +1324,10 @@
       <c r="E6" s="4"/>
       <c r="F6" s="86"/>
       <c r="G6" s="9" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1348,10 +1342,10 @@
       <c r="E7" s="4"/>
       <c r="F7" s="86"/>
       <c r="G7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -1366,7 +1360,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="7"/>
@@ -1386,10 +1380,10 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="5"/>
@@ -1404,7 +1398,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1420,7 +1414,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -1436,7 +1430,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -1452,7 +1446,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -1468,7 +1462,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -1484,13 +1478,13 @@
         <v>10</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
       <c r="K15" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L15" s="12"/>
     </row>
@@ -1502,13 +1496,13 @@
       <c r="E16" s="12"/>
       <c r="F16" s="88"/>
       <c r="G16" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="13" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="L16" s="12"/>
     </row>
@@ -1520,7 +1514,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="88"/>
       <c r="G17" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
@@ -1542,7 +1536,7 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L18" s="17"/>
     </row>
@@ -1558,7 +1552,7 @@
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L19" s="17"/>
     </row>
@@ -1574,7 +1568,7 @@
       <c r="I20" s="18"/>
       <c r="J20" s="18"/>
       <c r="K20" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L20" s="17"/>
     </row>
@@ -1590,12 +1584,12 @@
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
       <c r="I21" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J21" s="23"/>
       <c r="K21" s="20"/>
       <c r="L21" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
@@ -1616,12 +1610,12 @@
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J22" s="23"/>
       <c r="K22" s="20"/>
       <c r="L22" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M22" s="25"/>
       <c r="N22" s="25"/>
@@ -1645,7 +1639,7 @@
       <c r="J23" s="23"/>
       <c r="K23" s="23"/>
       <c r="L23" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M23" s="25"/>
       <c r="N23" s="25"/>
@@ -1669,7 +1663,7 @@
       <c r="J24" s="23"/>
       <c r="K24" s="23"/>
       <c r="L24" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M24" s="25"/>
       <c r="N24" s="25"/>
@@ -1698,8 +1692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADC453F-97E4-4EC8-8383-D8BA2226CD2D}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1716,51 +1710,51 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>46</v>
-      </c>
       <c r="H1" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="K1" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>88</v>
-      </c>
       <c r="L1" s="28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D2" s="84">
         <f xml:space="preserve"> SUM($H2:$T2)</f>
@@ -1776,13 +1770,13 @@
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D3" s="78">
         <f t="shared" ref="D3:D31" si="0" xml:space="preserve"> SUM($H3:$T3)</f>
@@ -1798,13 +1792,13 @@
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D4" s="78">
         <f t="shared" si="0"/>
@@ -1820,13 +1814,13 @@
     </row>
     <row r="5" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="78">
         <f t="shared" si="0"/>
@@ -1842,13 +1836,13 @@
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="78">
         <f t="shared" si="0"/>
@@ -1864,13 +1858,13 @@
     </row>
     <row r="7" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="72" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="78">
         <f t="shared" si="0"/>
@@ -1886,13 +1880,13 @@
     </row>
     <row r="8" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="72" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D8" s="78">
         <f t="shared" si="0"/>
@@ -1908,13 +1902,13 @@
     </row>
     <row r="9" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="78">
         <f t="shared" si="0"/>
@@ -1930,13 +1924,13 @@
     </row>
     <row r="10" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="78">
         <f t="shared" si="0"/>
@@ -1964,13 +1958,13 @@
     </row>
     <row r="11" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="79">
         <f t="shared" si="0"/>
@@ -1986,13 +1980,13 @@
     </row>
     <row r="12" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="79">
         <f t="shared" si="0"/>
@@ -2008,13 +2002,13 @@
     </row>
     <row r="13" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="79">
         <f t="shared" si="0"/>
@@ -2030,13 +2024,13 @@
     </row>
     <row r="14" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" s="73" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="79">
         <f t="shared" si="0"/>
@@ -2052,13 +2046,13 @@
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="79">
         <f t="shared" si="0"/>
@@ -2074,13 +2068,13 @@
     </row>
     <row r="16" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="79">
         <f t="shared" si="0"/>
@@ -2096,13 +2090,13 @@
     </row>
     <row r="17" spans="1:11" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="79">
         <f t="shared" si="0"/>
@@ -2118,13 +2112,13 @@
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="74" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="80">
         <f t="shared" si="0"/>
@@ -2140,13 +2134,13 @@
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19" s="74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="80">
         <f t="shared" si="0"/>
@@ -2162,13 +2156,13 @@
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="74" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="80">
         <f t="shared" si="0"/>
@@ -2184,13 +2178,13 @@
     </row>
     <row r="21" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="74" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="80">
         <f t="shared" si="0"/>
@@ -2206,13 +2200,13 @@
     </row>
     <row r="22" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="54" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" s="74" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="D22" s="80">
         <f t="shared" si="0"/>
@@ -2228,13 +2222,13 @@
     </row>
     <row r="23" spans="1:11" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" s="75" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="81">
         <f t="shared" si="0"/>
@@ -2250,13 +2244,13 @@
     </row>
     <row r="24" spans="1:11" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="81">
         <f t="shared" si="0"/>
@@ -2272,13 +2266,13 @@
     </row>
     <row r="25" spans="1:11" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="75" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" s="81">
         <f t="shared" si="0"/>
@@ -2294,13 +2288,13 @@
     </row>
     <row r="26" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B26" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D26" s="82">
         <f t="shared" si="0"/>
@@ -2316,13 +2310,13 @@
     </row>
     <row r="27" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B27" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" s="76" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D27" s="82">
         <f t="shared" si="0"/>
@@ -2338,13 +2332,13 @@
     </row>
     <row r="28" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="58" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B28" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28" s="76" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="82">
         <f t="shared" si="0"/>
@@ -2360,13 +2354,13 @@
     </row>
     <row r="29" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" s="76" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D29" s="82">
         <f t="shared" si="0"/>
@@ -2382,13 +2376,13 @@
     </row>
     <row r="30" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="58" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C30" s="76" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D30" s="82">
         <f t="shared" si="0"/>
@@ -2404,13 +2398,13 @@
     </row>
     <row r="31" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" s="77" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D31" s="83">
         <f t="shared" si="0"/>
@@ -2426,7 +2420,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C32" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D32" s="28">
         <f>SUM(D$2:D$31)</f>

</xml_diff>

<commit_message>
Changes for User Type Reduction
</commit_message>
<xml_diff>
--- a/docs/storyMap.xlsx
+++ b/docs/storyMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2020\CEN3031\project\career-finder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F685476-4F6D-49E2-A8B3-266D280975B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9490270A-FEB2-4B4F-BD46-9B702281C105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="careerFindStoryMap" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
   <si>
     <t>Base System</t>
   </si>
@@ -117,24 +117,9 @@
     <t>As a User after clicking on a celebrity link from an associated career page I would like to see that career's celebrity profile (name, photo, article) presented on a page.</t>
   </si>
   <si>
-    <t>As an Admin I would like to manage (CRUD) all user types (student, teacher, counselor, admin) from a listing of all users in the system.</t>
-  </si>
-  <si>
     <t>As an Admin I should be able to reset the password of any listed user in the system.</t>
   </si>
   <si>
-    <t>As a Teacher I want to manage (CRUD) students in my associated group (class).</t>
-  </si>
-  <si>
-    <t>As a Teacher I want to (CRUD) sub-groups (name, associated users) within my group (class).</t>
-  </si>
-  <si>
-    <t>As an Admin I want to manage (CRUD) groups (name, associated users) in the system.</t>
-  </si>
-  <si>
-    <t>As a Teacher I should be able to reset the password of students within my group (class).</t>
-  </si>
-  <si>
     <t>As a User I should be able to access the site with valid credentials (username/ password or e-mail/ password) from a login page.</t>
   </si>
   <si>
@@ -159,12 +144,6 @@
     <t>As a Student I should be able to bookmark careers I am interested in.</t>
   </si>
   <si>
-    <t>As a Teacher I can view point totals of students and student groups within my class.</t>
-  </si>
-  <si>
-    <t>As a Teacher I can reset point totals of students and groups within my class.</t>
-  </si>
-  <si>
     <t>As a Student I earn 1 point each time I visit a new career and all associated content.</t>
   </si>
   <si>
@@ -252,12 +231,6 @@
     <t>CF13</t>
   </si>
   <si>
-    <t>CF14</t>
-  </si>
-  <si>
-    <t>CF15</t>
-  </si>
-  <si>
     <t>CF16</t>
   </si>
   <si>
@@ -334,6 +307,21 @@
   </si>
   <si>
     <t>As a Student I want my response to be logged if it does not contain any known keywords so that my Counselor can improve the system.</t>
+  </si>
+  <si>
+    <t>As an Admin I would like to manage (CRUD) all user types (student, counselor, admin) from a listing of all users in the system.</t>
+  </si>
+  <si>
+    <t>As an Admin I want to manage (CRUD) classes (name, associated users) in the system.</t>
+  </si>
+  <si>
+    <t>As an Admin I want to be able to filter listed users by class.</t>
+  </si>
+  <si>
+    <t>As an Admin I can view point totals of students and classes containing students.</t>
+  </si>
+  <si>
+    <t>As an Admin I can reset point totals of individual students and all students within a particular class.</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,7 +1276,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>18</v>
@@ -1306,10 +1294,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="86"/>
       <c r="G5" s="9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -1324,7 +1312,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="86"/>
       <c r="G6" s="9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>19</v>
@@ -1380,10 +1368,10 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="10" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="5"/>
@@ -1398,7 +1386,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1414,7 +1402,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="10" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -1430,7 +1418,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="10" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -1440,33 +1428,39 @@
       <c r="A13" s="20"/>
       <c r="B13" s="17"/>
       <c r="C13" s="12"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="5"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="12"/>
     </row>
     <row r="14" spans="1:13" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="17"/>
       <c r="C14" s="12"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="5"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="L14" s="12"/>
     </row>
     <row r="15" spans="1:13" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
@@ -1474,53 +1468,49 @@
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
-      <c r="F15" s="88" t="s">
-        <v>10</v>
-      </c>
+      <c r="F15" s="88"/>
       <c r="G15" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="11"/>
-      <c r="K15" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="K15" s="16"/>
       <c r="L15" s="12"/>
     </row>
     <row r="16" spans="1:13" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20"/>
       <c r="B16" s="17"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="88"/>
-      <c r="G16" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="L16" s="12"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="17"/>
     </row>
     <row r="17" spans="1:20" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="17"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="88"/>
-      <c r="G17" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="12"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="17"/>
     </row>
     <row r="18" spans="1:20" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
@@ -1528,49 +1518,69 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="89" t="s">
-        <v>12</v>
-      </c>
+      <c r="F18" s="89"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
       <c r="K18" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L18" s="17"/>
     </row>
     <row r="19" spans="1:20" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="89"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="L19" s="17"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
     </row>
     <row r="20" spans="1:20" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="L20" s="17"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="23"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
     </row>
     <row r="21" spans="1:20" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="20"/>
@@ -1578,18 +1588,14 @@
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
-      <c r="F21" s="85" t="s">
-        <v>13</v>
-      </c>
+      <c r="F21" s="85"/>
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
-      <c r="I21" s="24" t="s">
-        <v>35</v>
-      </c>
+      <c r="I21" s="23"/>
       <c r="J21" s="23"/>
-      <c r="K21" s="20"/>
+      <c r="K21" s="23"/>
       <c r="L21" s="24" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
@@ -1609,13 +1615,11 @@
       <c r="F22" s="85"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
-      <c r="I22" s="24" t="s">
-        <v>36</v>
-      </c>
+      <c r="I22" s="23"/>
       <c r="J22" s="23"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="23"/>
       <c r="L22" s="24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="M22" s="25"/>
       <c r="N22" s="25"/>
@@ -1626,61 +1630,13 @@
       <c r="S22" s="25"/>
       <c r="T22" s="25"/>
     </row>
-    <row r="23" spans="1:20" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="M23" s="25"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="25"/>
-    </row>
-    <row r="24" spans="1:20" s="2" customFormat="1" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="25"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="F19:F22"/>
     <mergeCell ref="F4:F7"/>
-    <mergeCell ref="F9:F14"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F16:F18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -1690,10 +1646,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADC453F-97E4-4EC8-8383-D8BA2226CD2D}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,51 +1666,51 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G1" s="28" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J1" s="28" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D2" s="84">
         <f xml:space="preserve"> SUM($H2:$T2)</f>
@@ -1770,16 +1726,16 @@
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D3" s="78">
-        <f t="shared" ref="D3:D31" si="0" xml:space="preserve"> SUM($H3:$T3)</f>
+        <f t="shared" ref="D3:D29" si="0" xml:space="preserve"> SUM($H3:$T3)</f>
         <v>0</v>
       </c>
       <c r="E3" s="65"/>
@@ -1792,13 +1748,13 @@
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D4" s="78">
         <f t="shared" si="0"/>
@@ -1814,10 +1770,10 @@
     </row>
     <row r="5" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C5" s="72" t="s">
         <v>16</v>
@@ -1836,10 +1792,10 @@
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="50" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C6" s="72" t="s">
         <v>17</v>
@@ -1858,10 +1814,10 @@
     </row>
     <row r="7" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="50" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C7" s="72" t="s">
         <v>18</v>
@@ -1880,13 +1836,13 @@
     </row>
     <row r="8" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C8" s="72" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D8" s="78">
         <f t="shared" si="0"/>
@@ -1902,10 +1858,10 @@
     </row>
     <row r="9" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C9" s="72" t="s">
         <v>19</v>
@@ -1924,10 +1880,10 @@
     </row>
     <row r="10" spans="1:12" s="4" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C10" s="72" t="s">
         <v>20</v>
@@ -1958,13 +1914,13 @@
     </row>
     <row r="11" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="D11" s="79">
         <f t="shared" si="0"/>
@@ -1980,13 +1936,13 @@
     </row>
     <row r="12" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="79">
         <f t="shared" si="0"/>
@@ -2002,13 +1958,13 @@
     </row>
     <row r="13" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="52" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="D13" s="79">
         <f t="shared" si="0"/>
@@ -2024,13 +1980,13 @@
     </row>
     <row r="14" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="52" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C14" s="73" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="D14" s="79">
         <f t="shared" si="0"/>
@@ -2046,13 +2002,13 @@
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="79">
         <f t="shared" si="0"/>
@@ -2066,59 +2022,59 @@
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
     </row>
-    <row r="16" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="79">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="66"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-    </row>
-    <row r="17" spans="1:11" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="79">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="66"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
+    <row r="16" spans="1:12" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="80">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="67"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="80">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="67"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C18" s="74" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D18" s="80">
         <f t="shared" si="0"/>
@@ -2134,13 +2090,13 @@
     </row>
     <row r="19" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C19" s="74" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" s="80">
         <f t="shared" si="0"/>
@@ -2156,13 +2112,13 @@
     </row>
     <row r="20" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="54" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C20" s="74" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="D20" s="80">
         <f t="shared" si="0"/>
@@ -2176,59 +2132,59 @@
       <c r="J20" s="31"/>
       <c r="K20" s="31"/>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="74" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="80">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="67"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="31"/>
-    </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="54" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="74" t="s">
-        <v>93</v>
-      </c>
-      <c r="D22" s="80">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="67"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
+    <row r="21" spans="1:11" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="75" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="68"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+    </row>
+    <row r="22" spans="1:11" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="81">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="68"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
     </row>
     <row r="23" spans="1:11" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C23" s="75" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D23" s="81">
         <f t="shared" si="0"/>
@@ -2242,59 +2198,59 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="75" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="81">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="68"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-    </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="81">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="68"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
+    <row r="24" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="76" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="69"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+    </row>
+    <row r="25" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="76" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="82">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="69"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
     </row>
     <row r="26" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="58" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B26" s="44" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C26" s="76" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D26" s="82">
         <f t="shared" si="0"/>
@@ -2310,13 +2266,13 @@
     </row>
     <row r="27" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="58" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B27" s="44" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C27" s="76" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D27" s="82">
         <f t="shared" si="0"/>
@@ -2332,13 +2288,13 @@
     </row>
     <row r="28" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="58" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B28" s="44" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C28" s="76" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D28" s="82">
         <f t="shared" si="0"/>
@@ -2352,89 +2308,45 @@
       <c r="J28" s="33"/>
       <c r="K28" s="33"/>
     </row>
-    <row r="29" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="B29" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="76" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="82">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="69"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="59"/>
+    <row r="29" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="83">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="70"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="63"/>
       <c r="H29" s="33"/>
       <c r="I29" s="33"/>
       <c r="J29" s="33"/>
       <c r="K29" s="33"/>
     </row>
-    <row r="30" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="82">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="69"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-    </row>
-    <row r="31" spans="1:11" s="20" customFormat="1" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="61" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="77" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="83">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="70"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="28">
-        <f>SUM(D$2:D$31)</f>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="28">
+        <f>SUM(D$2:D$29)</f>
         <v>6</v>
       </c>
-      <c r="E32" s="28">
-        <f t="shared" ref="E32:G32" si="1">SUM(E$2:E$31)</f>
+      <c r="E30" s="28">
+        <f t="shared" ref="E30:G30" si="1">SUM(E$2:E$29)</f>
         <v>6</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F30" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="28">
+      <c r="G30" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Final Sprint 1 Story Map and Backlog
</commit_message>
<xml_diff>
--- a/docs/storyMap.xlsx
+++ b/docs/storyMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2020\CEN3031\project\career-finder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37361AAC-70AD-4A6B-B7E2-F9F8B42C34E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAA5166-7A59-4A31-B3A5-E9822B9C2301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -273,9 +273,6 @@
     <t>API</t>
   </si>
   <si>
-    <t>As a User after clicking on a career name I want to see base career data (name, salary, key subjects, description) and keyword-associated content links presented on a page.</t>
-  </si>
-  <si>
     <t>As an Admin I want to manage (CRUD) classes (name, associated users) in the system.</t>
   </si>
   <si>
@@ -300,18 +297,12 @@
     <t>As an Admin I want to manage (CRUD) the carrer clusters ( name, icon, keyword associations) displayed on the site.</t>
   </si>
   <si>
-    <t>As an Admin I want to manage (CRUD) the keywords (name, type: subject, interest) used to associate career clusters, careers, and celebrities.</t>
-  </si>
-  <si>
     <t>As an Admin I want to manage (CRUD) careers (name, salary, description, keyword associations) displayed on the site.</t>
   </si>
   <si>
     <t>As an Admin I want to manage (CRUD) Day-In-the-Life articles that are associated with careers.</t>
   </si>
   <si>
-    <t>As an Admin I want to manage (CRUD) the celebrity profiles (name, photo, article, keyword associations) displayed on the site.</t>
-  </si>
-  <si>
     <t>As an Admin I would like to manage (CRUD) all user types (student, admin) from a listing of all users in the system.</t>
   </si>
   <si>
@@ -331,6 +322,15 @@
   </si>
   <si>
     <t>CF15</t>
+  </si>
+  <si>
+    <t>As an Admin I want to manage (CRUD) the keywords (name, type: subject, interest) associated with career clusters and careers.</t>
+  </si>
+  <si>
+    <t>As an Admin I want to manage (CRUD) the celebrity profiles (name, photo, article) associated with careers.</t>
+  </si>
+  <si>
+    <t>As a User after clicking on a career name I want to see base career data (name, salary, subject keywords, description) and associated DITL/ Celebrity links presented on a page.</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>16</v>
@@ -1303,10 +1303,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="86"/>
       <c r="G5" s="9" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -1321,7 +1321,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="86"/>
       <c r="G6" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>17</v>
@@ -1339,7 +1339,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="86"/>
       <c r="G7" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>18</v>
@@ -1357,7 +1357,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="9" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="7"/>
@@ -1377,7 +1377,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>20</v>
@@ -1411,7 +1411,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -1427,7 +1427,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -1443,7 +1443,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -1461,13 +1461,13 @@
       <c r="E14" s="12"/>
       <c r="F14" s="88"/>
       <c r="G14" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L14" s="12"/>
     </row>
@@ -1479,7 +1479,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="88"/>
       <c r="G15" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -1549,7 +1549,7 @@
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
       <c r="I19" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J19" s="23"/>
       <c r="K19" s="20"/>
@@ -1575,7 +1575,7 @@
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
       <c r="I20" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J20" s="23"/>
       <c r="K20" s="20"/>
@@ -1658,7 +1658,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1719,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="84">
         <f xml:space="preserve"> SUM($H2:$T2)</f>
@@ -1741,7 +1741,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D3" s="78">
         <f t="shared" ref="D3:D29" si="0" xml:space="preserve"> SUM($H3:$T3)</f>
@@ -1763,7 +1763,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" s="78">
         <f t="shared" si="0"/>
@@ -1785,7 +1785,7 @@
         <v>29</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="78">
         <f t="shared" si="0"/>
@@ -1807,7 +1807,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="D6" s="78">
         <f t="shared" si="0"/>
@@ -1851,7 +1851,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="72" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="D8" s="78">
         <f t="shared" si="0"/>
@@ -1929,7 +1929,7 @@
         <v>37</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D11" s="79">
         <f t="shared" si="0"/>
@@ -1973,7 +1973,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="79">
         <f t="shared" si="0"/>
@@ -1995,7 +1995,7 @@
         <v>37</v>
       </c>
       <c r="C14" s="73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="79">
         <f t="shared" si="0"/>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>37</v>
@@ -2033,13 +2033,13 @@
     </row>
     <row r="16" spans="1:12" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B16" s="40" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="80">
         <f t="shared" si="0"/>
@@ -2061,7 +2061,7 @@
         <v>38</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D17" s="80">
         <f t="shared" si="0"/>
@@ -2083,7 +2083,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="80">
         <f t="shared" si="0"/>
@@ -2127,7 +2127,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="80">
         <f t="shared" si="0"/>
@@ -2215,7 +2215,7 @@
         <v>40</v>
       </c>
       <c r="C24" s="76" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="82">
         <f t="shared" si="0"/>
@@ -2237,7 +2237,7 @@
         <v>40</v>
       </c>
       <c r="C25" s="76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="82">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
updated storyMap based on Sprint 1 demo feedback
</commit_message>
<xml_diff>
--- a/docs/storyMap.xlsx
+++ b/docs/storyMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2020\CEN3031\project\career-finder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAA5166-7A59-4A31-B3A5-E9822B9C2301}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFAAE8E-38DE-41A4-AD6E-6B864E50BCA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1185" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="careerFindStoryMap" sheetId="1" r:id="rId1"/>
@@ -33,24 +33,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={EC7DB265-F8E0-4255-88FD-7E3B798F812B}</author>
-  </authors>
-  <commentList>
-    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{EC7DB265-F8E0-4255-88FD-7E3B798F812B}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    userRequirements &gt; 1. Base System: A content management system allowing users to … read… celebrity names, articles, photos.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
   <si>
@@ -297,9 +279,6 @@
     <t>As an Admin I want to manage (CRUD) the carrer clusters ( name, icon, keyword associations) displayed on the site.</t>
   </si>
   <si>
-    <t>As an Admin I want to manage (CRUD) careers (name, salary, description, keyword associations) displayed on the site.</t>
-  </si>
-  <si>
     <t>As an Admin I want to manage (CRUD) Day-In-the-Life articles that are associated with careers.</t>
   </si>
   <si>
@@ -324,13 +303,16 @@
     <t>CF15</t>
   </si>
   <si>
-    <t>As an Admin I want to manage (CRUD) the keywords (name, type: subject, interest) associated with career clusters and careers.</t>
-  </si>
-  <si>
     <t>As an Admin I want to manage (CRUD) the celebrity profiles (name, photo, article) associated with careers.</t>
   </si>
   <si>
     <t>As a User after clicking on a career name I want to see base career data (name, salary, subject keywords, description) and associated DITL/ Celebrity links presented on a page.</t>
+  </si>
+  <si>
+    <t>As an Admin I want to manage (CRUD) the keywords (name, type: subject, interest) associated with career clusters.</t>
+  </si>
+  <si>
+    <t>As an Admin I want to manage (CRUD) careers (name, salary, description) displayed on the site.</t>
   </si>
 </sst>
 </file>
@@ -928,9 +910,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Caplin,Robert O,II" id="{AEABF0B4-0D92-49F5-9F95-0526D087F34F}" userId="Caplin,Robert O,II" providerId="None"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1194,20 +1174,12 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H7" dT="2020-02-29T17:07:01.72" personId="{AEABF0B4-0D92-49F5-9F95-0526D087F34F}" id="{EC7DB265-F8E0-4255-88FD-7E3B798F812B}">
-    <text>userRequirements &gt; 1. Base System: A content management system allowing users to … read… celebrity names, articles, photos.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,10 +1275,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="86"/>
       <c r="G5" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>92</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -1321,7 +1293,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="86"/>
       <c r="G6" s="9" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>17</v>
@@ -1339,7 +1311,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="86"/>
       <c r="G7" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>18</v>
@@ -1357,7 +1329,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="7"/>
@@ -1377,7 +1349,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>20</v>
@@ -1443,7 +1415,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -1461,7 +1433,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="88"/>
       <c r="G14" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
@@ -1479,7 +1451,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="88"/>
       <c r="G15" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -1649,7 +1621,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1657,8 +1628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADC453F-97E4-4EC8-8383-D8BA2226CD2D}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,7 +1712,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D3" s="78">
         <f t="shared" ref="D3:D29" si="0" xml:space="preserve"> SUM($H3:$T3)</f>
@@ -1763,7 +1734,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="D4" s="78">
         <f t="shared" si="0"/>
@@ -1785,7 +1756,7 @@
         <v>29</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="78">
         <f t="shared" si="0"/>
@@ -1807,7 +1778,7 @@
         <v>29</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" s="78">
         <f t="shared" si="0"/>
@@ -1851,7 +1822,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="72" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D8" s="78">
         <f t="shared" si="0"/>
@@ -1929,7 +1900,7 @@
         <v>37</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="79">
         <f t="shared" si="0"/>
@@ -2011,7 +1982,7 @@
     </row>
     <row r="15" spans="1:12" s="5" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>37</v>
@@ -2033,7 +2004,7 @@
     </row>
     <row r="16" spans="1:12" s="12" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="40" t="s">
         <v>38</v>
@@ -2061,7 +2032,7 @@
         <v>38</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="80">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Noted potentially redundant test cases.
</commit_message>
<xml_diff>
--- a/docs/storyMap.xlsx
+++ b/docs/storyMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\UF\ufCompSciOnline\spring2020\CEN3031\project\career-finder\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE90DBBA-A02D-40BF-B097-8B09C642C1ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B099E04-F865-4534-A928-D962EE1B2477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="1890" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="careerFindStoryMap" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,112 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>user</author>
+  </authors>
+  <commentList>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{52ACFC18-55D0-42BF-9412-7EE33542DA90}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>rcaplin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+May be covered by CF01 TC.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{583C764B-F8B7-4AB5-85E7-BF42C5CCF0FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>rcaplin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+May be covered by CF10.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{88D88C29-8625-481D-B5D0-11F7C01C046A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>rcaplin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+May be covered by CF10.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{920A0DFC-2D6C-4CDC-A473-ADE8FE8633A5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>rcaplin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+May be covered by CF10.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
   <si>
@@ -319,7 +425,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,8 +470,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,6 +521,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -641,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -891,6 +1016,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1621,11 +1749,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADC453F-97E4-4EC8-8383-D8BA2226CD2D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADC453F-97E4-4EC8-8383-D8BA2226CD2D}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,7 +1859,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="51"/>
-      <c r="H3" s="29">
+      <c r="H3" s="90">
         <v>1</v>
       </c>
       <c r="I3" s="29">
@@ -2031,7 +2159,7 @@
         <v>8</v>
       </c>
       <c r="G12" s="53"/>
-      <c r="H12" s="30">
+      <c r="H12" s="90">
         <v>1</v>
       </c>
       <c r="I12" s="30">
@@ -2064,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="G13" s="53"/>
-      <c r="H13" s="30">
+      <c r="H13" s="90">
         <v>1</v>
       </c>
       <c r="I13" s="30">
@@ -2097,7 +2225,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="53"/>
-      <c r="H14" s="30">
+      <c r="H14" s="90">
         <v>1</v>
       </c>
       <c r="I14" s="30">
@@ -2476,5 +2604,6 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>